<commit_message>
Changes of mid day 4th Sept
</commit_message>
<xml_diff>
--- a/RiskFactors1July.xlsx
+++ b/RiskFactors1July.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48322b5fca08d482/GitHub/RiskFactorsLRGV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="925" documentId="8_{BF53BB47-CAD3-5447-80B1-DB3EADC3B8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F554CFC-F433-664E-953C-07EF0994B257}"/>
+  <xr:revisionPtr revIDLastSave="1034" documentId="8_{BF53BB47-CAD3-5447-80B1-DB3EADC3B8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1ABACC30-B889-0B4B-9A1F-C720EF0CF747}"/>
   <bookViews>
     <workbookView xWindow="13780" yWindow="460" windowWidth="25220" windowHeight="19660" activeTab="5" xr2:uid="{1AFF54DA-C0AD-1B48-BACA-D3A2AFC69637}"/>
   </bookViews>
@@ -25345,7 +25345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE5B4E5-3308-F04D-ADDE-6138069D962A}">
   <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ12" workbookViewId="0">
+    <sheetView topLeftCell="AZ1" workbookViewId="0">
       <selection activeCell="BT14" sqref="BT14"/>
     </sheetView>
   </sheetViews>
@@ -33455,8 +33455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F61359-DFAC-3947-A0D1-8BCB87E53ABD}">
   <dimension ref="A1:BO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BI37" sqref="BI37"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33708,16 +33708,16 @@
         <v>156</v>
       </c>
       <c r="N2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="P2" t="s">
         <v>170</v>
       </c>
       <c r="Q2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="R2" t="s">
         <v>156</v>
@@ -33774,7 +33774,7 @@
         <v>198</v>
       </c>
       <c r="AJ2" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK2" t="s">
         <v>207</v>
@@ -33911,16 +33911,16 @@
         <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="O3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="P3" t="s">
         <v>168</v>
       </c>
       <c r="Q3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="R3" t="s">
         <v>156</v>
@@ -33977,7 +33977,7 @@
         <v>199</v>
       </c>
       <c r="AJ3" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK3" t="s">
         <v>207</v>
@@ -34114,16 +34114,16 @@
         <v>85</v>
       </c>
       <c r="N4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="O4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="P4" t="s">
         <v>169</v>
       </c>
       <c r="Q4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="R4" t="s">
         <v>156</v>
@@ -34180,7 +34180,7 @@
         <v>199</v>
       </c>
       <c r="AJ4" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK4" t="s">
         <v>207</v>
@@ -34317,16 +34317,16 @@
         <v>156</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="O5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P5" t="s">
         <v>170</v>
       </c>
       <c r="Q5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="R5" t="s">
         <v>157</v>
@@ -34383,7 +34383,7 @@
         <v>198</v>
       </c>
       <c r="AJ5" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK5" t="s">
         <v>207</v>
@@ -34520,16 +34520,16 @@
         <v>157</v>
       </c>
       <c r="N6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="O6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P6" t="s">
         <v>168</v>
       </c>
       <c r="Q6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="R6" t="s">
         <v>156</v>
@@ -34586,7 +34586,7 @@
         <v>198</v>
       </c>
       <c r="AJ6" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK6" t="s">
         <v>207</v>
@@ -34723,16 +34723,16 @@
         <v>157</v>
       </c>
       <c r="N7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="O7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="P7" t="s">
         <v>170</v>
       </c>
       <c r="Q7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R7" t="s">
         <v>156</v>
@@ -34789,7 +34789,7 @@
         <v>199</v>
       </c>
       <c r="AJ7" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="AK7" t="s">
         <v>207</v>
@@ -34926,16 +34926,16 @@
         <v>156</v>
       </c>
       <c r="N8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="O8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="P8" t="s">
         <v>170</v>
       </c>
-      <c r="Q8" t="s">
-        <v>165</v>
+      <c r="Q8" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R8" t="s">
         <v>156</v>
@@ -34992,7 +34992,7 @@
         <v>198</v>
       </c>
       <c r="AJ8" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK8" t="s">
         <v>207</v>
@@ -35129,16 +35129,16 @@
         <v>157</v>
       </c>
       <c r="N9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="O9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="P9" t="s">
         <v>170</v>
       </c>
-      <c r="Q9" t="s">
-        <v>166</v>
+      <c r="Q9" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R9" t="s">
         <v>157</v>
@@ -35195,7 +35195,7 @@
         <v>197</v>
       </c>
       <c r="AJ9" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK9" t="s">
         <v>206</v>
@@ -35332,16 +35332,16 @@
         <v>157</v>
       </c>
       <c r="N10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P10" t="s">
         <v>169</v>
       </c>
       <c r="Q10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R10" t="s">
         <v>156</v>
@@ -35398,7 +35398,7 @@
         <v>199</v>
       </c>
       <c r="AJ10" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK10" t="s">
         <v>207</v>
@@ -35535,16 +35535,16 @@
         <v>157</v>
       </c>
       <c r="N11" t="s">
-        <v>165</v>
-      </c>
-      <c r="O11" t="s">
-        <v>165</v>
+        <v>156</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="P11" t="s">
         <v>168</v>
       </c>
-      <c r="Q11" t="s">
-        <v>165</v>
+      <c r="Q11" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R11" t="s">
         <v>156</v>
@@ -35601,7 +35601,7 @@
         <v>198</v>
       </c>
       <c r="AJ11" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK11" t="s">
         <v>208</v>
@@ -35738,16 +35738,16 @@
         <v>156</v>
       </c>
       <c r="N12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P12" t="s">
         <v>163</v>
       </c>
-      <c r="Q12" t="s">
-        <v>166</v>
+      <c r="Q12" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R12" t="s">
         <v>157</v>
@@ -35804,7 +35804,7 @@
         <v>198</v>
       </c>
       <c r="AJ12" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK12" t="s">
         <v>208</v>
@@ -35941,16 +35941,16 @@
         <v>156</v>
       </c>
       <c r="N13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P13" t="s">
         <v>168</v>
       </c>
       <c r="Q13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R13" t="s">
         <v>156</v>
@@ -36007,7 +36007,7 @@
         <v>199</v>
       </c>
       <c r="AJ13" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK13" t="s">
         <v>207</v>
@@ -36144,16 +36144,16 @@
         <v>157</v>
       </c>
       <c r="N14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="O14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P14" t="s">
         <v>170</v>
       </c>
       <c r="Q14" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R14" t="s">
         <v>156</v>
@@ -36210,7 +36210,7 @@
         <v>198</v>
       </c>
       <c r="AJ14" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK14" t="s">
         <v>207</v>
@@ -36347,16 +36347,16 @@
         <v>156</v>
       </c>
       <c r="N15" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="O15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P15" t="s">
         <v>168</v>
       </c>
-      <c r="Q15" t="s">
-        <v>167</v>
+      <c r="Q15" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R15" t="s">
         <v>156</v>
@@ -36413,7 +36413,7 @@
         <v>198</v>
       </c>
       <c r="AJ15" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK15" t="s">
         <v>207</v>
@@ -36550,16 +36550,16 @@
         <v>156</v>
       </c>
       <c r="N16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="P16" t="s">
         <v>163</v>
       </c>
-      <c r="Q16" t="s">
-        <v>165</v>
+      <c r="Q16" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R16" t="s">
         <v>156</v>
@@ -36616,7 +36616,7 @@
         <v>198</v>
       </c>
       <c r="AJ16" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK16" t="s">
         <v>208</v>
@@ -36753,16 +36753,16 @@
         <v>157</v>
       </c>
       <c r="N17" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O17" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P17" t="s">
         <v>168</v>
       </c>
-      <c r="Q17" t="s">
-        <v>166</v>
+      <c r="Q17" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R17" t="s">
         <v>157</v>
@@ -36819,7 +36819,7 @@
         <v>199</v>
       </c>
       <c r="AJ17" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="AK17" t="s">
         <v>208</v>
@@ -36956,16 +36956,16 @@
         <v>157</v>
       </c>
       <c r="N18" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O18" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P18" t="s">
         <v>168</v>
       </c>
-      <c r="Q18" t="s">
-        <v>165</v>
+      <c r="Q18" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R18" t="s">
         <v>156</v>
@@ -37022,7 +37022,7 @@
         <v>198</v>
       </c>
       <c r="AJ18" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK18" t="s">
         <v>207</v>
@@ -37159,16 +37159,16 @@
         <v>157</v>
       </c>
       <c r="N19" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="O19" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="P19" t="s">
         <v>170</v>
       </c>
-      <c r="Q19" t="s">
-        <v>165</v>
+      <c r="Q19" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R19" t="s">
         <v>157</v>
@@ -37225,7 +37225,7 @@
         <v>199</v>
       </c>
       <c r="AJ19" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK19" t="s">
         <v>208</v>
@@ -37362,16 +37362,16 @@
         <v>156</v>
       </c>
       <c r="N20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P20" t="s">
         <v>168</v>
       </c>
-      <c r="Q20" t="s">
-        <v>166</v>
+      <c r="Q20" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R20" t="s">
         <v>157</v>
@@ -37428,7 +37428,7 @@
         <v>198</v>
       </c>
       <c r="AJ20" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK20" t="s">
         <v>208</v>
@@ -37565,16 +37565,16 @@
         <v>157</v>
       </c>
       <c r="N21" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O21" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="P21" t="s">
         <v>170</v>
       </c>
-      <c r="Q21" t="s">
-        <v>166</v>
+      <c r="Q21" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R21" t="s">
         <v>156</v>
@@ -37631,7 +37631,7 @@
         <v>200</v>
       </c>
       <c r="AJ21" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="AK21" t="s">
         <v>208</v>
@@ -37768,16 +37768,16 @@
         <v>157</v>
       </c>
       <c r="N22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P22" t="s">
         <v>168</v>
       </c>
-      <c r="Q22" t="s">
-        <v>165</v>
+      <c r="Q22" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R22" t="s">
         <v>156</v>
@@ -37834,7 +37834,7 @@
         <v>199</v>
       </c>
       <c r="AJ22" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK22" t="s">
         <v>207</v>
@@ -37971,16 +37971,16 @@
         <v>157</v>
       </c>
       <c r="N23" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O23" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P23" t="s">
         <v>169</v>
       </c>
-      <c r="Q23" t="s">
-        <v>165</v>
+      <c r="Q23" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R23" t="s">
         <v>157</v>
@@ -38037,7 +38037,7 @@
         <v>198</v>
       </c>
       <c r="AJ23" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="AK23" t="s">
         <v>208</v>
@@ -38174,16 +38174,16 @@
         <v>156</v>
       </c>
       <c r="N24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P24" t="s">
         <v>169</v>
       </c>
-      <c r="Q24" t="s">
-        <v>165</v>
+      <c r="Q24" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R24" t="s">
         <v>157</v>
@@ -38240,7 +38240,7 @@
         <v>198</v>
       </c>
       <c r="AJ24" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="AK24" t="s">
         <v>208</v>
@@ -38377,16 +38377,16 @@
         <v>156</v>
       </c>
       <c r="N25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O25" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="P25" t="s">
         <v>170</v>
       </c>
       <c r="Q25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R25" t="s">
         <v>156</v>
@@ -38443,7 +38443,7 @@
         <v>198</v>
       </c>
       <c r="AJ25" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK25" t="s">
         <v>207</v>
@@ -38580,16 +38580,16 @@
         <v>157</v>
       </c>
       <c r="N26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P26" t="s">
         <v>168</v>
       </c>
-      <c r="Q26" t="s">
-        <v>165</v>
+      <c r="Q26" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R26" t="s">
         <v>156</v>
@@ -38646,7 +38646,7 @@
         <v>198</v>
       </c>
       <c r="AJ26" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="AK26" t="s">
         <v>207</v>
@@ -38783,16 +38783,16 @@
         <v>157</v>
       </c>
       <c r="N27" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O27" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P27" t="s">
         <v>169</v>
       </c>
       <c r="Q27" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R27" t="s">
         <v>157</v>
@@ -38849,7 +38849,7 @@
         <v>198</v>
       </c>
       <c r="AJ27" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="AK27" t="s">
         <v>208</v>
@@ -38986,16 +38986,16 @@
         <v>157</v>
       </c>
       <c r="N28" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="O28" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P28" t="s">
         <v>168</v>
       </c>
       <c r="Q28" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R28" t="s">
         <v>156</v>
@@ -39052,7 +39052,7 @@
         <v>197</v>
       </c>
       <c r="AJ28" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK28" t="s">
         <v>208</v>
@@ -39189,16 +39189,16 @@
         <v>157</v>
       </c>
       <c r="N29" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O29" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P29" t="s">
         <v>170</v>
       </c>
-      <c r="Q29" t="s">
-        <v>167</v>
+      <c r="Q29" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R29" t="s">
         <v>157</v>
@@ -39255,7 +39255,7 @@
         <v>198</v>
       </c>
       <c r="AJ29" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK29" t="s">
         <v>207</v>
@@ -39392,16 +39392,16 @@
         <v>157</v>
       </c>
       <c r="N30" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O30" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P30" t="s">
         <v>170</v>
       </c>
       <c r="Q30" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R30" t="s">
         <v>156</v>
@@ -39458,7 +39458,7 @@
         <v>198</v>
       </c>
       <c r="AJ30" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK30" t="s">
         <v>207</v>
@@ -39595,16 +39595,16 @@
         <v>157</v>
       </c>
       <c r="N31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P31" t="s">
         <v>170</v>
       </c>
       <c r="Q31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R31" t="s">
         <v>156</v>
@@ -39661,7 +39661,7 @@
         <v>198</v>
       </c>
       <c r="AJ31" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="AK31" t="s">
         <v>207</v>
@@ -39798,16 +39798,16 @@
         <v>157</v>
       </c>
       <c r="N32" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="O32" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="P32" t="s">
         <v>170</v>
       </c>
-      <c r="Q32" t="s">
-        <v>167</v>
+      <c r="Q32" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R32" t="s">
         <v>156</v>
@@ -39864,7 +39864,7 @@
         <v>198</v>
       </c>
       <c r="AJ32" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="AK32" t="s">
         <v>207</v>
@@ -39970,8 +39970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EF0E5C-921C-EB4F-B778-F5A9CD54BD2A}">
   <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="BI42" sqref="BI42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changes mid day Sept 4
</commit_message>
<xml_diff>
--- a/RiskFactors1July.xlsx
+++ b/RiskFactors1July.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48322b5fca08d482/GitHub/RiskFactorsLRGV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1034" documentId="8_{BF53BB47-CAD3-5447-80B1-DB3EADC3B8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1ABACC30-B889-0B4B-9A1F-C720EF0CF747}"/>
+  <xr:revisionPtr revIDLastSave="1145" documentId="8_{BF53BB47-CAD3-5447-80B1-DB3EADC3B8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C65215C-4049-4844-A984-765DD5F71431}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="460" windowWidth="25220" windowHeight="19660" activeTab="5" xr2:uid="{1AFF54DA-C0AD-1B48-BACA-D3A2AFC69637}"/>
+    <workbookView xWindow="13780" yWindow="460" windowWidth="25220" windowHeight="19660" activeTab="1" xr2:uid="{1AFF54DA-C0AD-1B48-BACA-D3A2AFC69637}"/>
   </bookViews>
   <sheets>
     <sheet name="ID" sheetId="2" r:id="rId1"/>
@@ -1784,7 +1784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BB7169-615A-3846-80CA-341EC6AF934D}">
   <dimension ref="A1:BS40"/>
   <sheetViews>
-    <sheetView topLeftCell="BA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="BJ21" sqref="BJ21"/>
     </sheetView>
   </sheetViews>
@@ -33455,8 +33455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F61359-DFAC-3947-A0D1-8BCB87E53ABD}">
   <dimension ref="A1:BO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BK34" sqref="BK34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33708,16 +33708,16 @@
         <v>156</v>
       </c>
       <c r="N2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O2" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="P2" t="s">
         <v>170</v>
       </c>
       <c r="Q2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="R2" t="s">
         <v>156</v>
@@ -33774,7 +33774,7 @@
         <v>198</v>
       </c>
       <c r="AJ2" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK2" t="s">
         <v>207</v>
@@ -33911,16 +33911,16 @@
         <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="O3" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="P3" t="s">
         <v>168</v>
       </c>
       <c r="Q3" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="R3" t="s">
         <v>156</v>
@@ -33977,7 +33977,7 @@
         <v>199</v>
       </c>
       <c r="AJ3" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK3" t="s">
         <v>207</v>
@@ -34114,16 +34114,16 @@
         <v>85</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="O4" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="P4" t="s">
         <v>169</v>
       </c>
       <c r="Q4" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="R4" t="s">
         <v>156</v>
@@ -34180,7 +34180,7 @@
         <v>199</v>
       </c>
       <c r="AJ4" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK4" t="s">
         <v>207</v>
@@ -34317,16 +34317,16 @@
         <v>156</v>
       </c>
       <c r="N5" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O5" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="P5" t="s">
         <v>170</v>
       </c>
       <c r="Q5" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="R5" t="s">
         <v>157</v>
@@ -34383,7 +34383,7 @@
         <v>198</v>
       </c>
       <c r="AJ5" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK5" t="s">
         <v>207</v>
@@ -34520,16 +34520,16 @@
         <v>157</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O6" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P6" t="s">
         <v>168</v>
       </c>
       <c r="Q6" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="R6" t="s">
         <v>156</v>
@@ -34586,7 +34586,7 @@
         <v>198</v>
       </c>
       <c r="AJ6" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK6" t="s">
         <v>207</v>
@@ -34723,16 +34723,16 @@
         <v>157</v>
       </c>
       <c r="N7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="O7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="P7" t="s">
         <v>170</v>
       </c>
       <c r="Q7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R7" t="s">
         <v>156</v>
@@ -34789,7 +34789,7 @@
         <v>199</v>
       </c>
       <c r="AJ7" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="AK7" t="s">
         <v>207</v>
@@ -34926,16 +34926,16 @@
         <v>156</v>
       </c>
       <c r="N8" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="P8" t="s">
         <v>170</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>156</v>
+      <c r="Q8" t="s">
+        <v>165</v>
       </c>
       <c r="R8" t="s">
         <v>156</v>
@@ -34992,7 +34992,7 @@
         <v>198</v>
       </c>
       <c r="AJ8" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK8" t="s">
         <v>207</v>
@@ -35129,16 +35129,16 @@
         <v>157</v>
       </c>
       <c r="N9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="O9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="P9" t="s">
         <v>170</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>156</v>
+      <c r="Q9" t="s">
+        <v>166</v>
       </c>
       <c r="R9" t="s">
         <v>157</v>
@@ -35195,7 +35195,7 @@
         <v>197</v>
       </c>
       <c r="AJ9" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK9" t="s">
         <v>206</v>
@@ -35332,16 +35332,16 @@
         <v>157</v>
       </c>
       <c r="N10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P10" t="s">
         <v>169</v>
       </c>
       <c r="Q10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R10" t="s">
         <v>156</v>
@@ -35398,7 +35398,7 @@
         <v>199</v>
       </c>
       <c r="AJ10" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK10" t="s">
         <v>207</v>
@@ -35535,16 +35535,16 @@
         <v>157</v>
       </c>
       <c r="N11" t="s">
-        <v>156</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>156</v>
+        <v>165</v>
+      </c>
+      <c r="O11" t="s">
+        <v>165</v>
       </c>
       <c r="P11" t="s">
         <v>168</v>
       </c>
-      <c r="Q11" s="4" t="s">
-        <v>156</v>
+      <c r="Q11" t="s">
+        <v>165</v>
       </c>
       <c r="R11" t="s">
         <v>156</v>
@@ -35601,7 +35601,7 @@
         <v>198</v>
       </c>
       <c r="AJ11" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK11" t="s">
         <v>208</v>
@@ -35738,16 +35738,16 @@
         <v>156</v>
       </c>
       <c r="N12" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O12" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P12" t="s">
         <v>163</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>156</v>
+      <c r="Q12" t="s">
+        <v>166</v>
       </c>
       <c r="R12" t="s">
         <v>157</v>
@@ -35804,7 +35804,7 @@
         <v>198</v>
       </c>
       <c r="AJ12" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK12" t="s">
         <v>208</v>
@@ -35941,16 +35941,16 @@
         <v>156</v>
       </c>
       <c r="N13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P13" t="s">
         <v>168</v>
       </c>
       <c r="Q13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R13" t="s">
         <v>156</v>
@@ -36007,7 +36007,7 @@
         <v>199</v>
       </c>
       <c r="AJ13" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK13" t="s">
         <v>207</v>
@@ -36144,16 +36144,16 @@
         <v>157</v>
       </c>
       <c r="N14" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O14" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="P14" t="s">
         <v>170</v>
       </c>
       <c r="Q14" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R14" t="s">
         <v>156</v>
@@ -36210,7 +36210,7 @@
         <v>198</v>
       </c>
       <c r="AJ14" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK14" t="s">
         <v>207</v>
@@ -36347,16 +36347,16 @@
         <v>156</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="O15" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P15" t="s">
         <v>168</v>
       </c>
-      <c r="Q15" s="4" t="s">
-        <v>156</v>
+      <c r="Q15" t="s">
+        <v>167</v>
       </c>
       <c r="R15" t="s">
         <v>156</v>
@@ -36413,7 +36413,7 @@
         <v>198</v>
       </c>
       <c r="AJ15" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK15" t="s">
         <v>207</v>
@@ -36550,16 +36550,16 @@
         <v>156</v>
       </c>
       <c r="N16" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O16" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="P16" t="s">
         <v>163</v>
       </c>
-      <c r="Q16" s="4" t="s">
-        <v>156</v>
+      <c r="Q16" t="s">
+        <v>165</v>
       </c>
       <c r="R16" t="s">
         <v>156</v>
@@ -36616,7 +36616,7 @@
         <v>198</v>
       </c>
       <c r="AJ16" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK16" t="s">
         <v>208</v>
@@ -36753,16 +36753,16 @@
         <v>157</v>
       </c>
       <c r="N17" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O17" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P17" t="s">
         <v>168</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>156</v>
+      <c r="Q17" t="s">
+        <v>166</v>
       </c>
       <c r="R17" t="s">
         <v>157</v>
@@ -36819,7 +36819,7 @@
         <v>199</v>
       </c>
       <c r="AJ17" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="AK17" t="s">
         <v>208</v>
@@ -36956,16 +36956,16 @@
         <v>157</v>
       </c>
       <c r="N18" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O18" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P18" t="s">
         <v>168</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>156</v>
+      <c r="Q18" t="s">
+        <v>165</v>
       </c>
       <c r="R18" t="s">
         <v>156</v>
@@ -37022,7 +37022,7 @@
         <v>198</v>
       </c>
       <c r="AJ18" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK18" t="s">
         <v>207</v>
@@ -37159,16 +37159,16 @@
         <v>157</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="O19" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="P19" t="s">
         <v>170</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>156</v>
+      <c r="Q19" t="s">
+        <v>165</v>
       </c>
       <c r="R19" t="s">
         <v>157</v>
@@ -37225,7 +37225,7 @@
         <v>199</v>
       </c>
       <c r="AJ19" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK19" t="s">
         <v>208</v>
@@ -37362,16 +37362,16 @@
         <v>156</v>
       </c>
       <c r="N20" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O20" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P20" t="s">
         <v>168</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>156</v>
+      <c r="Q20" t="s">
+        <v>166</v>
       </c>
       <c r="R20" t="s">
         <v>157</v>
@@ -37428,7 +37428,7 @@
         <v>198</v>
       </c>
       <c r="AJ20" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK20" t="s">
         <v>208</v>
@@ -37565,16 +37565,16 @@
         <v>157</v>
       </c>
       <c r="N21" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O21" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="P21" t="s">
         <v>170</v>
       </c>
-      <c r="Q21" s="4" t="s">
-        <v>156</v>
+      <c r="Q21" t="s">
+        <v>166</v>
       </c>
       <c r="R21" t="s">
         <v>156</v>
@@ -37631,7 +37631,7 @@
         <v>200</v>
       </c>
       <c r="AJ21" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="AK21" t="s">
         <v>208</v>
@@ -37768,16 +37768,16 @@
         <v>157</v>
       </c>
       <c r="N22" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O22" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P22" t="s">
         <v>168</v>
       </c>
-      <c r="Q22" s="4" t="s">
-        <v>156</v>
+      <c r="Q22" t="s">
+        <v>165</v>
       </c>
       <c r="R22" t="s">
         <v>156</v>
@@ -37834,7 +37834,7 @@
         <v>199</v>
       </c>
       <c r="AJ22" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK22" t="s">
         <v>207</v>
@@ -37971,16 +37971,16 @@
         <v>157</v>
       </c>
       <c r="N23" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O23" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P23" t="s">
         <v>169</v>
       </c>
-      <c r="Q23" s="4" t="s">
-        <v>156</v>
+      <c r="Q23" t="s">
+        <v>165</v>
       </c>
       <c r="R23" t="s">
         <v>157</v>
@@ -38037,7 +38037,7 @@
         <v>198</v>
       </c>
       <c r="AJ23" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="AK23" t="s">
         <v>208</v>
@@ -38174,16 +38174,16 @@
         <v>156</v>
       </c>
       <c r="N24" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O24" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P24" t="s">
         <v>169</v>
       </c>
-      <c r="Q24" s="4" t="s">
-        <v>156</v>
+      <c r="Q24" t="s">
+        <v>165</v>
       </c>
       <c r="R24" t="s">
         <v>157</v>
@@ -38240,7 +38240,7 @@
         <v>198</v>
       </c>
       <c r="AJ24" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="AK24" t="s">
         <v>208</v>
@@ -38377,16 +38377,16 @@
         <v>156</v>
       </c>
       <c r="N25" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="P25" t="s">
         <v>170</v>
       </c>
       <c r="Q25" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R25" t="s">
         <v>156</v>
@@ -38443,7 +38443,7 @@
         <v>198</v>
       </c>
       <c r="AJ25" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK25" t="s">
         <v>207</v>
@@ -38580,16 +38580,16 @@
         <v>157</v>
       </c>
       <c r="N26" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O26" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P26" t="s">
         <v>168</v>
       </c>
-      <c r="Q26" s="4" t="s">
-        <v>156</v>
+      <c r="Q26" t="s">
+        <v>165</v>
       </c>
       <c r="R26" t="s">
         <v>156</v>
@@ -38646,7 +38646,7 @@
         <v>198</v>
       </c>
       <c r="AJ26" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="AK26" t="s">
         <v>207</v>
@@ -38783,16 +38783,16 @@
         <v>157</v>
       </c>
       <c r="N27" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O27" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P27" t="s">
         <v>169</v>
       </c>
       <c r="Q27" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R27" t="s">
         <v>157</v>
@@ -38849,7 +38849,7 @@
         <v>198</v>
       </c>
       <c r="AJ27" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="AK27" t="s">
         <v>208</v>
@@ -38986,16 +38986,16 @@
         <v>157</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O28" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="P28" t="s">
         <v>168</v>
       </c>
       <c r="Q28" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R28" t="s">
         <v>156</v>
@@ -39052,7 +39052,7 @@
         <v>197</v>
       </c>
       <c r="AJ28" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK28" t="s">
         <v>208</v>
@@ -39189,16 +39189,16 @@
         <v>157</v>
       </c>
       <c r="N29" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O29" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P29" t="s">
         <v>170</v>
       </c>
-      <c r="Q29" s="4" t="s">
-        <v>156</v>
+      <c r="Q29" t="s">
+        <v>167</v>
       </c>
       <c r="R29" t="s">
         <v>157</v>
@@ -39255,7 +39255,7 @@
         <v>198</v>
       </c>
       <c r="AJ29" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK29" t="s">
         <v>207</v>
@@ -39392,16 +39392,16 @@
         <v>157</v>
       </c>
       <c r="N30" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O30" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P30" t="s">
         <v>170</v>
       </c>
       <c r="Q30" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R30" t="s">
         <v>156</v>
@@ -39458,7 +39458,7 @@
         <v>198</v>
       </c>
       <c r="AJ30" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK30" t="s">
         <v>207</v>
@@ -39595,16 +39595,16 @@
         <v>157</v>
       </c>
       <c r="N31" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O31" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P31" t="s">
         <v>170</v>
       </c>
       <c r="Q31" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R31" t="s">
         <v>156</v>
@@ -39661,7 +39661,7 @@
         <v>198</v>
       </c>
       <c r="AJ31" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="AK31" t="s">
         <v>207</v>
@@ -39798,16 +39798,16 @@
         <v>157</v>
       </c>
       <c r="N32" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O32" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P32" t="s">
         <v>170</v>
       </c>
-      <c r="Q32" s="4" t="s">
-        <v>156</v>
+      <c r="Q32" t="s">
+        <v>167</v>
       </c>
       <c r="R32" t="s">
         <v>156</v>
@@ -39864,7 +39864,7 @@
         <v>198</v>
       </c>
       <c r="AJ32" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="AK32" t="s">
         <v>207</v>
@@ -39970,8 +39970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EF0E5C-921C-EB4F-B778-F5A9CD54BD2A}">
   <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="BI42" sqref="BI42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BQ11" sqref="BQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>